<commit_message>
Updated documentation and added some comments.
Signed-off-by: Cristi Iacob <cristiiacob98@gmail.com>
</commit_message>
<xml_diff>
--- a/dokumentation/Lab01_ReviewReport.xlsx
+++ b/dokumentation/Lab01_ReviewReport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\facultate\sem5\proiect colectiv\business-management-backend\dokumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38026461-A87C-4DE7-A062-D4BFF0B39CAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26640" windowHeight="10755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="89">
   <si>
     <t>Nr.</t>
   </si>
@@ -183,9 +184,6 @@
     <t>Layering is logically inconsistent</t>
   </si>
   <si>
-    <t>No error handling strategies</t>
-  </si>
-  <si>
     <t>No design patterns used</t>
   </si>
   <si>
@@ -271,9 +269,6 @@
 illogical comments</t>
   </si>
   <si>
-    <t>equivalence sign (==) instead of strict equivalence sign(===)</t>
-  </si>
-  <si>
     <t>Document  Title:</t>
   </si>
   <si>
@@ -300,12 +295,15 @@
   </si>
   <si>
     <t>Requirements Phase Defects Checklist</t>
+  </si>
+  <si>
+    <t>No error handling strategies on lower architectural layers. Error handling only on requests layer.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -480,26 +478,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -510,6 +490,40 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -518,28 +532,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -816,10 +814,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -828,41 +826,41 @@
     <col min="2" max="2" width="38.140625" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="5.28515625" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" style="14" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="42.85546875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="10"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="10"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" ht="53.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -875,13 +873,13 @@
         <v>7</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="10"/>
+      <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
@@ -894,13 +892,13 @@
         <v>7</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -913,9 +911,9 @@
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="10"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -928,9 +926,9 @@
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="10"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" ht="51.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -943,13 +941,13 @@
         <v>7</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="10"/>
+      <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -962,13 +960,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="G8" s="10"/>
+      <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -981,63 +979,63 @@
         <v>7</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="10"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="s">
+      <c r="C14" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-    </row>
-    <row r="14" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="C15" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1045,11 +1043,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:F18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,34 +1058,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1100,8 +1098,8 @@
         <v>7</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="5"/>
+      <c r="F3" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1116,8 +1114,8 @@
       <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1130,8 +1128,8 @@
         <v>7</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -1144,8 +1142,8 @@
         <v>7</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -1158,9 +1156,9 @@
       <c r="D7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9" t="s">
-        <v>51</v>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1174,9 +1172,9 @@
       <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9" t="s">
-        <v>52</v>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1190,8 +1188,8 @@
         <v>7</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -1204,8 +1202,8 @@
         <v>7</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -1218,8 +1216,8 @@
         <v>7</v>
       </c>
       <c r="D11" s="4"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -1232,50 +1230,50 @@
         <v>7</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="22" t="s">
+      <c r="C17" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-    </row>
-    <row r="17" spans="2:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+      <c r="C18" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1294,11 +1292,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,252 +1307,250 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="17" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="18"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="20" t="s">
-        <v>79</v>
+      <c r="E3" s="5"/>
+      <c r="F3" s="11" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
     </row>
     <row r="6" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9" t="s">
-        <v>78</v>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
     </row>
     <row r="9" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="C10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9" t="s">
-        <v>77</v>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="9" t="s">
-        <v>80</v>
-      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="27.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
+      <c r="C19" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-    </row>
-    <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
+      <c r="C20" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="C19" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>